<commit_message>
blood glucose -> blood sugar
</commit_message>
<xml_diff>
--- a/mapping/mml4_flowsheet.xlsx
+++ b/mapping/mml4_flowsheet.xlsx
@@ -958,13 +958,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Blood glucose(itemName="Blood glucose"の場合）</t>
-    <rPh sb="39" eb="41">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>itemName="Blood glucose"の場合</t>
     <rPh sb="25" eb="27">
       <t>バアイ</t>
@@ -1738,6 +1731,13 @@
   </si>
   <si>
     <t>/content[openEHR-EHR-EVALUATION.clinical_synopsis.v1]/data[at0001]/items[at0002]/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Blood sugar(itemName="Blood sugar"の場合）</t>
+    <rPh sb="35" eb="37">
+      <t>バアイ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2392,8 +2392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
+      <selection activeCell="A212" sqref="A212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2438,7 +2438,7 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2450,7 +2450,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2462,7 +2462,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
@@ -2471,20 +2471,20 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="H4" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>295</v>
-      </c>
       <c r="J4" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -2494,20 +2494,20 @@
       </c>
       <c r="F5" s="3"/>
       <c r="H5" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -2521,7 +2521,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
@@ -2544,7 +2544,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
@@ -2558,17 +2558,17 @@
         <v>55</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -2583,17 +2583,17 @@
         <v>58</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
@@ -2605,7 +2605,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
@@ -2628,7 +2628,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
@@ -2639,20 +2639,20 @@
       </c>
       <c r="F12" s="3"/>
       <c r="H12" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="I12" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>295</v>
-      </c>
       <c r="J12" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>10</v>
@@ -2664,20 +2664,20 @@
         <v>24</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>10</v>
@@ -2689,7 +2689,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
@@ -2712,7 +2712,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
@@ -2723,20 +2723,20 @@
       </c>
       <c r="F16" s="3"/>
       <c r="H16" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>10</v>
@@ -2749,17 +2749,17 @@
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>10</v>
@@ -2771,7 +2771,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.15">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.15">
@@ -2811,7 +2811,7 @@
         <v>1.3</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2825,10 +2825,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>230</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>231</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13" t="s">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>233</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>234</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13" t="s">
@@ -2863,10 +2863,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>236</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13" t="s">
@@ -2876,7 +2876,7 @@
         <v>7</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -2884,10 +2884,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>238</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>239</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13" t="s">
@@ -2903,10 +2903,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>240</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>241</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13" t="s">
@@ -2922,10 +2922,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>242</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>243</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13" t="s">
@@ -2941,10 +2941,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" s="35" t="s">
         <v>244</v>
-      </c>
-      <c r="B28" s="35" t="s">
-        <v>245</v>
       </c>
       <c r="C28" s="35"/>
       <c r="D28" s="35" t="s">
@@ -2963,7 +2963,7 @@
         <v>1.4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2977,7 +2977,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
@@ -2985,16 +2985,16 @@
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.15">
@@ -3002,7 +3002,7 @@
         <v>85</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
@@ -3013,13 +3013,13 @@
       </c>
       <c r="F31" s="3"/>
       <c r="H31" t="s">
+        <v>315</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>317</v>
-      </c>
       <c r="J31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.15">
@@ -3027,7 +3027,7 @@
         <v>87</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
@@ -3037,10 +3037,10 @@
         <v>7</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
@@ -3048,7 +3048,7 @@
         <v>90</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
@@ -3059,13 +3059,13 @@
       </c>
       <c r="F33" s="3"/>
       <c r="H33" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.15">
@@ -3073,7 +3073,7 @@
         <v>92</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
@@ -3084,21 +3084,21 @@
       </c>
       <c r="F34" s="3"/>
       <c r="H34" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J34" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
@@ -3109,21 +3109,21 @@
       </c>
       <c r="F35" s="3"/>
       <c r="H35" t="s">
+        <v>360</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="J35" t="s">
         <v>361</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="J35" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
@@ -3134,21 +3134,21 @@
       </c>
       <c r="F36" s="3"/>
       <c r="H36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J36" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
@@ -3159,21 +3159,21 @@
       </c>
       <c r="F37" s="3"/>
       <c r="H37" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J37" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
@@ -3184,21 +3184,21 @@
       </c>
       <c r="F38" s="3"/>
       <c r="H38" t="s">
+        <v>366</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="J38" t="s">
         <v>367</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="J38" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -3209,10 +3209,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>265</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
@@ -3223,21 +3223,21 @@
       </c>
       <c r="F40" s="3"/>
       <c r="H40" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I40" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="J40" t="s">
         <v>371</v>
-      </c>
-      <c r="J40" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>266</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
@@ -3248,21 +3248,21 @@
       </c>
       <c r="F41" s="3"/>
       <c r="H41" t="s">
+        <v>373</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="J41" t="s">
         <v>374</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="J41" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>268</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>269</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
@@ -3273,21 +3273,21 @@
       </c>
       <c r="F42" s="3"/>
       <c r="H42" t="s">
+        <v>375</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="J42" t="s">
         <v>377</v>
-      </c>
-      <c r="J42" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>271</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
@@ -3298,13 +3298,13 @@
       </c>
       <c r="F43" s="3"/>
       <c r="H43" t="s">
+        <v>378</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="J43" t="s">
         <v>379</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="J43" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.15">
@@ -3312,7 +3312,7 @@
         <v>1.5</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
@@ -3323,18 +3323,18 @@
       </c>
       <c r="F44" s="3"/>
       <c r="H44" t="s">
+        <v>380</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="J44" t="s">
         <v>381</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="J44" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3364,7 +3364,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A49" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>6</v>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A50" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B50" s="13" t="s">
         <v>9</v>
@@ -3404,7 +3404,7 @@
         <v>57</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K50" s="15"/>
     </row>
@@ -3429,7 +3429,7 @@
         <v>60</v>
       </c>
       <c r="J51" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K51" s="15"/>
     </row>
@@ -3452,7 +3452,7 @@
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K52" s="15"/>
     </row>
@@ -3469,13 +3469,13 @@
       </c>
       <c r="I53" s="14"/>
       <c r="J53" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K53" s="15"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>16</v>
@@ -3496,7 +3496,7 @@
         <v>62</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K54" s="15"/>
     </row>
@@ -3523,7 +3523,7 @@
         <v>62</v>
       </c>
       <c r="J55" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K55" s="15"/>
     </row>
@@ -3544,7 +3544,7 @@
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K56" s="15"/>
     </row>
@@ -3561,13 +3561,13 @@
       </c>
       <c r="I57" s="14"/>
       <c r="J57" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K57" s="15"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A58" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>22</v>
@@ -3588,7 +3588,7 @@
         <v>57</v>
       </c>
       <c r="J58" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K58" s="15"/>
     </row>
@@ -3615,7 +3615,7 @@
         <v>60</v>
       </c>
       <c r="J59" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K59" s="15"/>
     </row>
@@ -3636,7 +3636,7 @@
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
       <c r="J60" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K60" s="15"/>
     </row>
@@ -3653,13 +3653,13 @@
       </c>
       <c r="I61" s="14"/>
       <c r="J61" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K61" s="15"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A62" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>27</v>
@@ -3680,7 +3680,7 @@
         <v>62</v>
       </c>
       <c r="J62" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K62" s="15"/>
     </row>
@@ -3705,7 +3705,7 @@
         <v>62</v>
       </c>
       <c r="J63" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K63" s="15"/>
     </row>
@@ -3726,7 +3726,7 @@
       <c r="H64" s="14"/>
       <c r="I64" s="14"/>
       <c r="J64" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K64" s="15"/>
     </row>
@@ -3743,13 +3743,13 @@
       </c>
       <c r="I65" s="14"/>
       <c r="J65" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K65" s="15"/>
     </row>
     <row r="66" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B66" s="24" t="s">
         <v>94</v>
@@ -3770,7 +3770,7 @@
         <v>62</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K66" s="19"/>
     </row>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A70" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>33</v>
@@ -3844,7 +3844,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A71" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>36</v>
@@ -3865,7 +3865,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A72" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>38</v>
@@ -3886,13 +3886,13 @@
         <v>65</v>
       </c>
       <c r="J72" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K72" s="15"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A73" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>41</v>
@@ -3917,7 +3917,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A74" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>44</v>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A75" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>46</v>
@@ -3958,7 +3958,7 @@
       <c r="G75" s="14"/>
       <c r="H75" s="14"/>
       <c r="I75" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J75" s="14" t="s">
         <v>77</v>
@@ -3967,7 +3967,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A76" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>48</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A77" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>50</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A78" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>86</v>
@@ -4040,7 +4040,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A79" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>88</v>
@@ -4063,7 +4063,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A80" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>91</v>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="81" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>93</v>
@@ -4111,7 +4111,7 @@
         <v>62</v>
       </c>
       <c r="J81" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K81" s="19"/>
     </row>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A85" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>33</v>
@@ -4162,7 +4162,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A86" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>36</v>
@@ -4182,7 +4182,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A87" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>38</v>
@@ -4208,7 +4208,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A88" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>41</v>
@@ -4232,7 +4232,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A89" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>44</v>
@@ -4253,12 +4253,12 @@
         <v>60</v>
       </c>
       <c r="J89" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A90" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B90" s="13" t="s">
         <v>46</v>
@@ -4272,7 +4272,7 @@
       <c r="G90" s="14"/>
       <c r="H90" s="14"/>
       <c r="I90" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J90" s="15" t="s">
         <v>79</v>
@@ -4280,7 +4280,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A91" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>48</v>
@@ -4298,7 +4298,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A92" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>50</v>
@@ -4318,7 +4318,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A93" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>86</v>
@@ -4344,7 +4344,7 @@
     </row>
     <row r="94" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A94" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>88</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A95" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B95" s="13" t="s">
         <v>91</v>
@@ -4392,7 +4392,7 @@
     </row>
     <row r="96" spans="1:11" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B96" s="17" t="s">
         <v>93</v>
@@ -4454,7 +4454,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A101" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B101" s="13" t="s">
         <v>33</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A102" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B102" s="13" t="s">
         <v>36</v>
@@ -4496,7 +4496,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A103" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B103" s="13" t="s">
         <v>38</v>
@@ -4522,7 +4522,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A104" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B104" s="13" t="s">
         <v>41</v>
@@ -4546,7 +4546,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A105" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B105" s="13" t="s">
         <v>44</v>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A106" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B106" s="13" t="s">
         <v>33</v>
@@ -4594,7 +4594,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A107" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B107" s="13" t="s">
         <v>36</v>
@@ -4614,7 +4614,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A108" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B108" s="13" t="s">
         <v>38</v>
@@ -4640,7 +4640,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A109" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B109" s="13" t="s">
         <v>41</v>
@@ -4664,7 +4664,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A110" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B110" s="13" t="s">
         <v>44</v>
@@ -4690,7 +4690,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A111" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B111" s="13" t="s">
         <v>46</v>
@@ -4704,7 +4704,7 @@
       <c r="G111" s="14"/>
       <c r="H111" s="14"/>
       <c r="I111" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J111" s="15" t="s">
         <v>117</v>
@@ -4712,7 +4712,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A112" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B112" s="13" t="s">
         <v>48</v>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A113" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B113" s="13" t="s">
         <v>50</v>
@@ -4756,7 +4756,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A114" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B114" s="13" t="s">
         <v>86</v>
@@ -4782,7 +4782,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A115" s="21" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B115" s="13" t="s">
         <v>88</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A116" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B116" s="13" t="s">
         <v>91</v>
@@ -4836,7 +4836,7 @@
     </row>
     <row r="117" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A117" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B117" s="17" t="s">
         <v>93</v>
@@ -4885,7 +4885,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A122" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B122" s="13" t="s">
         <v>33</v>
@@ -4907,7 +4907,7 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A123" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B123" s="13" t="s">
         <v>36</v>
@@ -4927,7 +4927,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A124" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B124" s="13" t="s">
         <v>38</v>
@@ -4953,7 +4953,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A125" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B125" s="13" t="s">
         <v>41</v>
@@ -4977,7 +4977,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A126" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B126" s="13" t="s">
         <v>44</v>
@@ -5003,7 +5003,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A127" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B127" s="13" t="s">
         <v>46</v>
@@ -5017,7 +5017,7 @@
       <c r="G127" s="14"/>
       <c r="H127" s="14"/>
       <c r="I127" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J127" s="15" t="s">
         <v>131</v>
@@ -5025,7 +5025,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A128" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B128" s="13" t="s">
         <v>48</v>
@@ -5043,7 +5043,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A129" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B129" s="13" t="s">
         <v>50</v>
@@ -5069,7 +5069,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A130" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B130" s="13" t="s">
         <v>86</v>
@@ -5095,7 +5095,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A131" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B131" s="13" t="s">
         <v>88</v>
@@ -5117,7 +5117,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A132" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B132" s="13" t="s">
         <v>91</v>
@@ -5138,12 +5138,12 @@
         <v>62</v>
       </c>
       <c r="J132" s="15" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="133" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A133" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B133" s="17" t="s">
         <v>93</v>
@@ -5164,7 +5164,7 @@
         <v>69</v>
       </c>
       <c r="J133" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="135" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -5340,7 +5340,7 @@
       <c r="G143" s="14"/>
       <c r="H143" s="14"/>
       <c r="I143" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J143" s="15" t="s">
         <v>84</v>
@@ -5413,7 +5413,7 @@
         <v>62</v>
       </c>
       <c r="J146" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.15">
@@ -5441,7 +5441,7 @@
         <v>62</v>
       </c>
       <c r="J147" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.15">
@@ -5467,7 +5467,7 @@
         <v>62</v>
       </c>
       <c r="J148" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="149" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -5493,7 +5493,7 @@
         <v>151</v>
       </c>
       <c r="J149" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="151" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -5653,7 +5653,7 @@
       <c r="G158" s="14"/>
       <c r="H158" s="14"/>
       <c r="I158" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J158" s="15" t="s">
         <v>84</v>
@@ -5726,7 +5726,7 @@
         <v>62</v>
       </c>
       <c r="J161" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.15">
@@ -5754,7 +5754,7 @@
         <v>62</v>
       </c>
       <c r="J162" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.15">
@@ -5780,7 +5780,7 @@
         <v>62</v>
       </c>
       <c r="J163" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="164" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -5806,7 +5806,7 @@
         <v>151</v>
       </c>
       <c r="J164" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="166" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -5966,7 +5966,7 @@
       <c r="G173" s="14"/>
       <c r="H173" s="14"/>
       <c r="I173" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J173" s="15" t="s">
         <v>84</v>
@@ -6039,7 +6039,7 @@
         <v>62</v>
       </c>
       <c r="J176" s="15" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.15">
@@ -6067,7 +6067,7 @@
         <v>62</v>
       </c>
       <c r="J177" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.15">
@@ -6093,7 +6093,7 @@
         <v>62</v>
       </c>
       <c r="J178" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="179" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -6119,7 +6119,7 @@
         <v>151</v>
       </c>
       <c r="J179" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="181" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -6279,7 +6279,7 @@
       <c r="G188" s="14"/>
       <c r="H188" s="14"/>
       <c r="I188" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J188" s="15" t="s">
         <v>169</v>
@@ -6426,7 +6426,7 @@
         <v>151</v>
       </c>
       <c r="J194" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="196" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -6586,7 +6586,7 @@
       <c r="G203" s="14"/>
       <c r="H203" s="14"/>
       <c r="I203" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J203" s="15" t="s">
         <v>180</v>
@@ -6738,7 +6738,7 @@
     </row>
     <row r="211" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A211" s="20" t="s">
-        <v>187</v>
+        <v>382</v>
       </c>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.15">
@@ -6776,7 +6776,7 @@
       </c>
       <c r="G213" s="14"/>
       <c r="H213" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I213" s="14"/>
       <c r="J213" s="15"/>
@@ -6818,13 +6818,13 @@
       <c r="F215" s="13"/>
       <c r="G215" s="14"/>
       <c r="H215" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I215" s="13" t="s">
         <v>81</v>
       </c>
       <c r="J215" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.15">
@@ -6848,7 +6848,7 @@
       <c r="H216" s="14"/>
       <c r="I216" s="14"/>
       <c r="J216" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.15">
@@ -6868,13 +6868,13 @@
       <c r="F217" s="13"/>
       <c r="G217" s="14"/>
       <c r="H217" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I217" s="13" t="s">
         <v>69</v>
       </c>
       <c r="J217" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.15">
@@ -6893,10 +6893,10 @@
       <c r="G218" s="14"/>
       <c r="H218" s="14"/>
       <c r="I218" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J218" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.15">
@@ -6940,7 +6940,7 @@
         <v>62</v>
       </c>
       <c r="J220" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.15">
@@ -6966,7 +6966,7 @@
         <v>62</v>
       </c>
       <c r="J221" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.15">
@@ -7008,13 +7008,13 @@
       <c r="F223" s="13"/>
       <c r="G223" s="14"/>
       <c r="H223" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I223" s="7" t="s">
         <v>62</v>
       </c>
       <c r="J223" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="224" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -7125,13 +7125,13 @@
       <c r="F230" s="13"/>
       <c r="G230" s="14"/>
       <c r="H230" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I230" s="13" t="s">
         <v>81</v>
       </c>
       <c r="J230" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.15">
@@ -7155,7 +7155,7 @@
       <c r="H231" s="14"/>
       <c r="I231" s="14"/>
       <c r="J231" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.15">
@@ -7175,13 +7175,13 @@
       <c r="F232" s="13"/>
       <c r="G232" s="14"/>
       <c r="H232" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I232" s="13" t="s">
         <v>69</v>
       </c>
       <c r="J232" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.15">
@@ -7200,10 +7200,10 @@
       <c r="G233" s="14"/>
       <c r="H233" s="14"/>
       <c r="I233" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J233" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.15">
@@ -7323,18 +7323,18 @@
       <c r="F239" s="17"/>
       <c r="G239" s="18"/>
       <c r="H239" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I239" s="18" t="s">
         <v>151</v>
       </c>
       <c r="J239" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="241" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A241" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.15">
@@ -7372,13 +7372,13 @@
       </c>
       <c r="G243" s="14"/>
       <c r="H243" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I243" s="7" t="s">
         <v>62</v>
       </c>
       <c r="J243" s="15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.15">
@@ -7398,13 +7398,13 @@
       <c r="F244" s="13"/>
       <c r="G244" s="14"/>
       <c r="H244" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I244" s="7" t="s">
         <v>62</v>
       </c>
       <c r="J244" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.15">
@@ -7424,13 +7424,13 @@
       <c r="F245" s="13"/>
       <c r="G245" s="14"/>
       <c r="H245" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I245" s="13" t="s">
         <v>81</v>
       </c>
       <c r="J245" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.15">
@@ -7454,7 +7454,7 @@
       <c r="H246" s="14"/>
       <c r="I246" s="14"/>
       <c r="J246" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.15">
@@ -7474,13 +7474,13 @@
       <c r="F247" s="13"/>
       <c r="G247" s="14"/>
       <c r="H247" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I247" s="13" t="s">
         <v>69</v>
       </c>
       <c r="J247" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.15">
@@ -7499,10 +7499,10 @@
       <c r="G248" s="14"/>
       <c r="H248" s="14"/>
       <c r="I248" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J248" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.15">
@@ -7546,7 +7546,7 @@
         <v>60</v>
       </c>
       <c r="J250" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.15">
@@ -7572,7 +7572,7 @@
         <v>62</v>
       </c>
       <c r="J251" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="252" spans="1:10" x14ac:dyDescent="0.15">
@@ -7614,13 +7614,13 @@
       <c r="F253" s="13"/>
       <c r="G253" s="14"/>
       <c r="H253" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I253" s="7" t="s">
         <v>62</v>
       </c>
       <c r="J253" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="254" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -7640,18 +7640,18 @@
       <c r="F254" s="17"/>
       <c r="G254" s="18"/>
       <c r="H254" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I254" s="18" t="s">
         <v>151</v>
       </c>
       <c r="J254" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="257" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A257" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.15">
@@ -7659,7 +7659,7 @@
         <v>1.3</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C258" s="9"/>
       <c r="D258" s="9"/>
@@ -7674,10 +7674,10 @@
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A259" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B259" s="13" t="s">
         <v>230</v>
-      </c>
-      <c r="B259" s="13" t="s">
-        <v>231</v>
       </c>
       <c r="C259" s="13"/>
       <c r="D259" s="13" t="s">
@@ -7685,25 +7685,25 @@
       </c>
       <c r="E259" s="13"/>
       <c r="F259" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G259" s="14"/>
       <c r="H259" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="I259" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="I259" s="13" t="s">
-        <v>314</v>
-      </c>
       <c r="J259" s="15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A260" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B260" s="13" t="s">
         <v>233</v>
-      </c>
-      <c r="B260" s="13" t="s">
-        <v>234</v>
       </c>
       <c r="C260" s="13"/>
       <c r="D260" s="13" t="s">
@@ -7715,21 +7715,21 @@
       <c r="F260" s="13"/>
       <c r="G260" s="14"/>
       <c r="H260" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="I260" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="I260" s="13" t="s">
-        <v>317</v>
-      </c>
       <c r="J260" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A261" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B261" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="B261" s="13" t="s">
-        <v>236</v>
       </c>
       <c r="C261" s="13"/>
       <c r="D261" s="13" t="s">
@@ -7739,21 +7739,21 @@
         <v>7</v>
       </c>
       <c r="F261" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G261" s="14"/>
       <c r="H261" s="14"/>
       <c r="I261" s="14"/>
       <c r="J261" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A262" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B262" s="13" t="s">
         <v>238</v>
-      </c>
-      <c r="B262" s="13" t="s">
-        <v>239</v>
       </c>
       <c r="C262" s="13"/>
       <c r="D262" s="13" t="s">
@@ -7765,21 +7765,21 @@
       <c r="F262" s="13"/>
       <c r="G262" s="14"/>
       <c r="H262" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="I262" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="I262" s="13" t="s">
+      <c r="J262" s="15" t="s">
         <v>320</v>
-      </c>
-      <c r="J262" s="15" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A263" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B263" s="13" t="s">
         <v>240</v>
-      </c>
-      <c r="B263" s="13" t="s">
-        <v>241</v>
       </c>
       <c r="C263" s="13"/>
       <c r="D263" s="13" t="s">
@@ -7791,21 +7791,21 @@
       <c r="F263" s="13"/>
       <c r="G263" s="14"/>
       <c r="H263" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I263" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J263" s="15" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A264" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B264" s="13" t="s">
         <v>242</v>
-      </c>
-      <c r="B264" s="13" t="s">
-        <v>243</v>
       </c>
       <c r="C264" s="13"/>
       <c r="D264" s="13" t="s">
@@ -7817,21 +7817,21 @@
       <c r="F264" s="13"/>
       <c r="G264" s="14"/>
       <c r="H264" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I264" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J264" s="15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="265" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A265" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B265" s="17" t="s">
         <v>244</v>
-      </c>
-      <c r="B265" s="17" t="s">
-        <v>245</v>
       </c>
       <c r="C265" s="17"/>
       <c r="D265" s="17" t="s">
@@ -7843,18 +7843,18 @@
       <c r="F265" s="17"/>
       <c r="G265" s="18"/>
       <c r="H265" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="I265" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="J265" s="19" t="s">
         <v>330</v>
-      </c>
-      <c r="I265" s="17" t="s">
-        <v>320</v>
-      </c>
-      <c r="J265" s="19" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="267" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A267" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.15">
@@ -7862,7 +7862,7 @@
         <v>1.3</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C268" s="9"/>
       <c r="D268" s="9"/>
@@ -7877,10 +7877,10 @@
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A269" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B269" s="13" t="s">
         <v>230</v>
-      </c>
-      <c r="B269" s="13" t="s">
-        <v>231</v>
       </c>
       <c r="C269" s="13"/>
       <c r="D269" s="13" t="s">
@@ -7888,25 +7888,25 @@
       </c>
       <c r="E269" s="13"/>
       <c r="F269" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G269" s="14"/>
       <c r="H269" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I269" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="I269" s="13" t="s">
-        <v>345</v>
-      </c>
       <c r="J269" s="15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A270" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B270" s="13" t="s">
         <v>233</v>
-      </c>
-      <c r="B270" s="13" t="s">
-        <v>234</v>
       </c>
       <c r="C270" s="13"/>
       <c r="D270" s="13" t="s">
@@ -7918,21 +7918,21 @@
       <c r="F270" s="13"/>
       <c r="G270" s="14"/>
       <c r="H270" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="I270" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="I270" s="13" t="s">
-        <v>317</v>
-      </c>
       <c r="J270" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A271" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B271" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="B271" s="13" t="s">
-        <v>236</v>
       </c>
       <c r="C271" s="13"/>
       <c r="D271" s="13" t="s">
@@ -7942,21 +7942,21 @@
         <v>7</v>
       </c>
       <c r="F271" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G271" s="14"/>
       <c r="H271" s="14"/>
       <c r="I271" s="14"/>
       <c r="J271" s="15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A272" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B272" s="13" t="s">
         <v>238</v>
-      </c>
-      <c r="B272" s="13" t="s">
-        <v>239</v>
       </c>
       <c r="C272" s="13"/>
       <c r="D272" s="13" t="s">
@@ -7968,21 +7968,21 @@
       <c r="F272" s="13"/>
       <c r="G272" s="14"/>
       <c r="H272" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="I272" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="I272" s="13" t="s">
-        <v>320</v>
-      </c>
       <c r="J272" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A273" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B273" s="13" t="s">
         <v>240</v>
-      </c>
-      <c r="B273" s="13" t="s">
-        <v>241</v>
       </c>
       <c r="C273" s="13"/>
       <c r="D273" s="13" t="s">
@@ -7994,21 +7994,21 @@
       <c r="F273" s="13"/>
       <c r="G273" s="14"/>
       <c r="H273" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I273" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="J273" s="15" t="s">
         <v>350</v>
-      </c>
-      <c r="J273" s="15" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A274" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B274" s="13" t="s">
         <v>242</v>
-      </c>
-      <c r="B274" s="13" t="s">
-        <v>243</v>
       </c>
       <c r="C274" s="13"/>
       <c r="D274" s="13" t="s">
@@ -8020,21 +8020,21 @@
       <c r="F274" s="13"/>
       <c r="G274" s="14"/>
       <c r="H274" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I274" s="13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J274" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="275" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A275" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B275" s="17" t="s">
         <v>244</v>
-      </c>
-      <c r="B275" s="17" t="s">
-        <v>245</v>
       </c>
       <c r="C275" s="17"/>
       <c r="D275" s="17" t="s">
@@ -8047,10 +8047,10 @@
       <c r="G275" s="18"/>
       <c r="H275" s="18"/>
       <c r="I275" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J275" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed blood glucose comment
</commit_message>
<xml_diff>
--- a/mapping/mml4_flowsheet.xlsx
+++ b/mapping/mml4_flowsheet.xlsx
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="384">
   <si>
     <t>Elements</t>
   </si>
@@ -1738,6 +1738,10 @@
   </si>
   <si>
     <t>/content[openEHR-EHR-EVALUATION.clinical_synopsis.v1]/data[at0001]/items[at0002]/value</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>/content[openEHR-EHR-SECTION.vital_signs.v1]/items[openEHR-EHR-OBSERVATION.lab_test-blood_glucose.v1]/data[at0001]/events[at0002]/data[at0003]/items[openEHR-EHR-CLUSTER.lab_result_annotation.v1]/items[at0017]/value</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -2392,8 +2396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="J225" sqref="J225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7040,7 +7044,7 @@
         <v>151</v>
       </c>
       <c r="J224" s="19" t="s">
-        <v>181</v>
+        <v>383</v>
       </c>
     </row>
     <row r="226" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">

</xml_diff>